<commit_message>
[docs] update STRIDE document
update STRIDE document
</commit_message>
<xml_diff>
--- a/docs/05_threat_modeling/jetsonNano_STRIDE.xlsx
+++ b/docs/05_threat_modeling/jetsonNano_STRIDE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\security\cmu\temp\cmu_project\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\security\cmu\temp\cmu_project\docs\05_threat_modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="179">
   <si>
     <t>Id</t>
   </si>
@@ -183,21 +183,12 @@
     <t>Elevation by Changing the Execution Flow in 1.1 Client (PC)</t>
   </si>
   <si>
-    <t>An attacker may pass data into 1.1 Client (PC) in order to change the flow of program execution within 1.1 Client (PC) to the attacker's choosing.</t>
-  </si>
-  <si>
     <t>1.1 Client (PC) May be Subject to Elevation of Privilege Using Remote Code Execution</t>
   </si>
   <si>
-    <t>2.1 Server (Jetson) may be able to remotely execute code for 1.1 Client (PC).</t>
-  </si>
-  <si>
     <t>Potential Process Crash or Stop for 1.1 Client (PC)</t>
   </si>
   <si>
-    <t>1.1 Client (PC) crashes, halts, stops or runs slowly; in all cases violating an availability metric.</t>
-  </si>
-  <si>
     <t>Potential Data Repudiation by 1.1 Client (PC)</t>
   </si>
   <si>
@@ -210,21 +201,6 @@
     <t>Spoofing the 1.1 Client (PC) Process</t>
   </si>
   <si>
-    <t>1.1 Client (PC) may be spoofed by an attacker and this may lead to information disclosure by 2.1 Server (Jetson). Consider using a standard authentication mechanism to identify the destination process.</t>
-  </si>
-  <si>
-    <t>2.1 Server (Jetson) may be spoofed by an attacker and this may lead to unauthorized access to 1.1 Client (PC). Consider using a standard authentication mechanism to identify the source process.</t>
-  </si>
-  <si>
-    <t>2.1 Server (Jetson) may be able to impersonate the context of 2.2 Face Recognition Module in order to gain additional privilege.</t>
-  </si>
-  <si>
-    <t>2.2 Face Recognition Module may be able to impersonate the context of 2.1 Server (Jetson) in order to gain additional privilege.</t>
-  </si>
-  <si>
-    <t>DF4.6 Face Reg. Meta Data</t>
-  </si>
-  <si>
     <t>Elevation by Changing the Execution Flow in 2.1 Server (Jetson)</t>
   </si>
   <si>
@@ -246,9 +222,6 @@
     <t>Potential Excessive Resource Consumption for 2.1 Server (Jetson) or S1. User Credential Data File System</t>
   </si>
   <si>
-    <t>Does 2.1 Server (Jetson) or S1. User Credential Data File System take explicit steps to control resource consumption? Resource consumption attacks can be hard to deal with, and there are times that it makes sense to let the OS do the job. Be careful that your resource requests don't deadlock, and that they do timeout.</t>
-  </si>
-  <si>
     <t>Weak Credential Storage</t>
   </si>
   <si>
@@ -264,9 +237,6 @@
     <t>Insufficient Auditing</t>
   </si>
   <si>
-    <t>Does the log capture enough data to understand what happened in the past? Do your logs capture enough data to understand an incident after the fact? Is such capture lightweight enough to be left on all the time? Do you have enough data to deal with repudiation claims? Make sure you log sufficient and appropriate data to handle a repudiation claims. You might want to talk to an audit expert as well as a privacy expert about your choice of data.</t>
-  </si>
-  <si>
     <t>3.1 Camera Unit may be able to remotely execute code for 2.1 Server (Jetson).</t>
   </si>
   <si>
@@ -276,9 +246,6 @@
     <t>Data Logs from an Unknown Source</t>
   </si>
   <si>
-    <t>Do you accept logs from unknown or weakly authenticated users or systems? Identify and authenticate the source of the logs before accepting them.</t>
-  </si>
-  <si>
     <t>Weak Access Control for a Resource</t>
   </si>
   <si>
@@ -342,16 +309,7 @@
     <t>DF2.5 Result (Video Stream...)</t>
   </si>
   <si>
-    <t>Data flowing across DF2.5 Result (Video Stream...) may be tampered with by an attacker. This may lead to a denial of service attack against 1.1 Client (PC) or an elevation of privilege attack against 1.1 Client (PC) or an information disclosure by 1.1 Client (PC). Failure to verify that input is as expected is a root cause of a very large number of exploitable issues. Consider all paths and the way they handle data. Verify that all input is verified for correctness using an approved list input validation approach.</t>
-  </si>
-  <si>
-    <t>Data flowing across DF2.5 Result (Video Stream...) may be sniffed by an attacker. Depending on what type of data an attacker can read, it may be used to attack other parts of the system or simply be a disclosure of information leading to compliance violations. Consider encrypting the data flow.</t>
-  </si>
-  <si>
     <t>Data Flow DF2.5 Result (Video Stream...) Is Potentially Interrupted</t>
-  </si>
-  <si>
-    <t>DF4.5 Sensor Data, Req. Ctrl</t>
   </si>
   <si>
     <t>[Threat] 
@@ -378,13 +336,6 @@
 #1. 2.1 Server (Jetson) may be able to remotely execute code for 3.1 Camera Unit
 [Review]
 #1.Camera is just simple unit, so no threat is expected to arise.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>[Threat] 
-#1. An external agent interrupts data flowing across a trust boundary in either direction.
-[Review]
-#1. Since they are connected by physical cables, it is difficult to interupt with data.</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -583,6 +534,228 @@
 An attacker modify user credential data and then server can use it without checking.
 [Review]
 Use hashing</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Review]
+Client cannot distinguish Human Users.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Review]
+#1. Since they are connected by physical cables, it is difficult to interrupt with data.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Threat] 
+#1. An external agent interrupts data flowing across a trust boundary in either direction.
+[Review]
+#1. Since they are connected by physical cables, it is difficult to interrupt with data.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DF3.2 Sensor Data</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Does 2.1 Server (Jetson) or S1. User Credential Data File System take explicit steps to control resource consumption? Resource consumption attacks can be hard to deal with, and there are times that it makes sense to let the OS do the job. Be careful that your resource requests don't deadlock, and that they do timeout.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[Threat]
+It is possible to add a lot of Images in the storage.
+[Review]
+The limitation of number of image is need. </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Security Requirement]
+#1. The number of images should be under 100.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Threat]
+User credential may be disclosed.
+[Review]
+User credential should be encrypted before being stored.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Does the log capture enough data to understand what happened in the past? Do your logs capture enough data to understand an incident after the fact? Is such capture lightweight enough to be left on all the time? Do you have enough data to deal with repudiation claims? Make sure you log sufficient and appropriate data to handle a repudiation claims. You might want to talk to an audit expert as well as a privacy expert about your choice of data.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Do you accept logs from unknown or weakly authenticated users or systems? Identify and authenticate the source of the logs before accepting them.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Review]
+This case will not happen in the system.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Review]
+This case will not happen in the system.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Threat] 
+User Credential Data can be exposed to attackers.
+[Review]
+User Credential Data should be kept securely.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Security Requirement]
+#1. This data should be encrypted.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.1 Server (Jetson) may be spoofed by an attacker and this may lead to unauthorized access to 1.1 Client (PC). Consider using a standard authentication mechanism to identify the source process.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Security Requirement]
+#1. Mutual authentication</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1 Client (PC) may be spoofed by an attacker and this may lead to information disclosure by 2.1 Server (Jetson). Consider using a standard authentication mechanism to identify the destination process.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Threat]
+Server (Jetson) may be spoofed by an attacker 
+[Review]
+use mutual authentication</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Threat]
+Client (PC) may be spoofed by an attacker 
+[Review]
+use mutual authentication</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data flowing across DF2.5 Result (Video Stream...) may be tampered with by an attacker. This may lead to a denial of service attack against 1.1 Client (PC) or an elevation of privilege attack against 1.1 Client (PC) or an information disclosure by 1.1 Client (PC). Failure to verify that input is as expected is a root cause of a very large number of exploitable issues. Consider all paths and the way they handle data. Verify that all input is verified for correctness using an approved list input validation approach.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[Threat]
+Video Stream may be tampered with by an attacker.
+[Review]
+Video Stream over the connection should be protected. 
+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Security Requirement]
+#1. need to TLS</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Review]
+even though This case will happen, this case does not affect .</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data flowing across DF2.5 Result (Video Stream...) may be sniffed by an attacker. Depending on what type of data an attacker can read, it may be used to attack other parts of the system or simply be a disclosure of information leading to compliance violations. Consider encrypting the data flow.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[Threat]
+Video Stream may be sniffed with by an attacker.
+[Review]
+Video Stream over the connection should be protected. 
+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1 Client (PC) crashes, halts, stops or runs slowly; in all cases violating an availability metric.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Security Requirement]
+#1. Server should be robust in abnormal case.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Threat]
+Client (PC) crashes, halts, stops or runs slowly.
+[Review]
+Server is working properly.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>An external agent interrupts data flowing across a trust boundary in either direction.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Threat]
+An external agent interrupts data flowing across a trust boundary in either direction.
+[Review]
+This case won't be handled.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Review]
+support only single user</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.1 Server (Jetson) may be able to remotely execute code for 1.1 Client (PC).</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Threat]
+Server (Jetson) may be able to remotely execute code
+[Review]
+need input sanitization</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Security Requirement]
+#1. need input sanitization</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>An attacker may pass data into 1.1 Client (PC) in order to change the flow of program execution within 1.1 Client (PC) to the attacker's choosing.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Threat]
+An attacker may pass data into 1.1 Client (PC)
+[Review]
+need input sanitization</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1543,10 +1716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="C50" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1594,13 +1767,13 @@
         <v>829</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>38</v>
@@ -1609,13 +1782,13 @@
         <v>11</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
@@ -1623,13 +1796,13 @@
         <v>827</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>38</v>
@@ -1638,13 +1811,13 @@
         <v>11</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="99" x14ac:dyDescent="0.3">
@@ -1652,13 +1825,13 @@
         <v>826</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>38</v>
@@ -1667,13 +1840,13 @@
         <v>11</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" ht="115.5" x14ac:dyDescent="0.3">
@@ -1687,7 +1860,7 @@
         <v>34</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>38</v>
@@ -1696,16 +1869,16 @@
         <v>11</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="132" x14ac:dyDescent="0.3">
@@ -1719,7 +1892,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>38</v>
@@ -1728,13 +1901,13 @@
         <v>11</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="J6" s="7"/>
     </row>
@@ -1749,7 +1922,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>38</v>
@@ -1761,10 +1934,10 @@
         <v>46</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="2" customFormat="1" ht="99" x14ac:dyDescent="0.3">
@@ -1778,7 +1951,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>38</v>
@@ -1787,16 +1960,16 @@
         <v>11</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="2" customFormat="1" ht="132" x14ac:dyDescent="0.3">
@@ -1810,7 +1983,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>38</v>
@@ -1822,13 +1995,13 @@
         <v>52</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" ht="115.5" x14ac:dyDescent="0.3">
@@ -1842,7 +2015,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>38</v>
@@ -1854,10 +2027,10 @@
         <v>43</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" ht="99" x14ac:dyDescent="0.3">
@@ -1865,13 +2038,13 @@
         <v>640</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>38</v>
@@ -1883,10 +2056,10 @@
         <v>19</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
@@ -1900,7 +2073,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>38</v>
@@ -1912,10 +2085,10 @@
         <v>40</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
@@ -1923,13 +2096,13 @@
         <v>642</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>38</v>
@@ -1938,13 +2111,13 @@
         <v>11</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" ht="99" x14ac:dyDescent="0.3">
@@ -1952,13 +2125,13 @@
         <v>643</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>38</v>
@@ -1967,16 +2140,16 @@
         <v>11</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
@@ -2002,10 +2175,10 @@
         <v>50</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="2" customFormat="1" ht="115.5" x14ac:dyDescent="0.3">
@@ -2031,13 +2204,13 @@
         <v>49</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="2" customFormat="1" ht="115.5" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="2" customFormat="1" ht="132" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>646</v>
       </c>
@@ -2060,10 +2233,10 @@
         <v>48</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
@@ -2089,10 +2262,10 @@
         <v>46</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
@@ -2118,10 +2291,10 @@
         <v>44</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
@@ -2147,10 +2320,10 @@
         <v>43</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="J20" s="3"/>
     </row>
@@ -2159,7 +2332,7 @@
         <v>651</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>18</v>
@@ -2174,13 +2347,13 @@
         <v>11</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="2" customFormat="1" ht="132" x14ac:dyDescent="0.3">
@@ -2203,13 +2376,13 @@
         <v>11</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="2" customFormat="1" ht="115.5" x14ac:dyDescent="0.3">
@@ -2217,7 +2390,7 @@
         <v>653</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>9</v>
@@ -2232,13 +2405,13 @@
         <v>11</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
@@ -2246,7 +2419,7 @@
         <v>654</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>9</v>
@@ -2261,13 +2434,13 @@
         <v>11</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
@@ -2293,10 +2466,10 @@
         <v>37</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
@@ -2322,13 +2495,13 @@
         <v>35</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="2" customFormat="1" ht="115.5" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="2" customFormat="1" ht="132" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>667</v>
       </c>
@@ -2351,10 +2524,10 @@
         <v>32</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
@@ -2380,13 +2553,13 @@
         <v>29</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>669</v>
       </c>
@@ -2409,10 +2582,10 @@
         <v>26</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
@@ -2438,10 +2611,10 @@
         <v>21</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="2" customFormat="1" ht="115.5" x14ac:dyDescent="0.3">
@@ -2467,10 +2640,10 @@
         <v>19</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="2" customFormat="1" ht="132" x14ac:dyDescent="0.3">
@@ -2496,13 +2669,13 @@
         <v>12</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="2" customFormat="1" ht="115.5" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="2" customFormat="1" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>674</v>
       </c>
@@ -2525,13 +2698,13 @@
         <v>16</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>675</v>
       </c>
@@ -2554,611 +2727,669 @@
         <v>14</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="6">
         <v>847</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="2" customFormat="1" ht="132" x14ac:dyDescent="0.3">
+      <c r="A36" s="6">
+        <v>845</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A37" s="6">
+        <v>842</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="2" customFormat="1" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A38" s="6">
+        <v>841</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A39" s="6">
+        <v>840</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C39" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="6">
+        <v>839</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="A41" s="6">
+        <v>837</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="6">
+        <v>836</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A43" s="6">
+        <v>691</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="A44" s="6">
+        <v>692</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="A45" s="6">
+        <v>695</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="A46" s="6">
+        <v>696</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="2" customFormat="1" ht="132" x14ac:dyDescent="0.3">
+      <c r="A47" s="6">
+        <v>697</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A48" s="6">
+        <v>698</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A49" s="6">
+        <v>699</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="A50" s="6">
+        <v>700</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-    </row>
-    <row r="36" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="4">
-        <v>845</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="D50" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A51" s="6">
+        <v>701</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="A52" s="6">
+        <v>702</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="A53" s="6">
+        <v>703</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="I53" s="6"/>
+      <c r="J53" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="A54" s="6">
+        <v>704</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="I54" s="6"/>
+      <c r="J54" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="2" customFormat="1" ht="99" x14ac:dyDescent="0.3">
+      <c r="A55" s="6">
+        <v>898</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-    </row>
-    <row r="37" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="4">
-        <v>842</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-    </row>
-    <row r="38" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="4">
-        <v>841</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-    </row>
-    <row r="39" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A39" s="4">
-        <v>840</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-    </row>
-    <row r="40" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A40" s="4">
-        <v>839</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-    </row>
-    <row r="41" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A41" s="4">
-        <v>837</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-    </row>
-    <row r="42" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
-        <v>836</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-    </row>
-    <row r="43" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="4">
-        <v>691</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-    </row>
-    <row r="44" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A44" s="4">
-        <v>692</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-    </row>
-    <row r="45" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A45" s="4">
-        <v>695</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-    </row>
-    <row r="46" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A46" s="4">
-        <v>696</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-    </row>
-    <row r="47" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A47" s="4">
-        <v>697</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-    </row>
-    <row r="48" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A48" s="4">
-        <v>698</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-    </row>
-    <row r="49" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A49" s="4">
-        <v>699</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C49" s="4" t="s">
+      <c r="D55" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" s="2" customFormat="1" ht="99" x14ac:dyDescent="0.3">
+      <c r="A56" s="6">
+        <v>897</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-    </row>
-    <row r="50" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A50" s="4">
-        <v>700</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-    </row>
-    <row r="51" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A51" s="4">
-        <v>701</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-    </row>
-    <row r="52" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A52" s="4">
-        <v>702</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-    </row>
-    <row r="53" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A53" s="4">
-        <v>703</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-    </row>
-    <row r="54" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A54" s="4">
-        <v>704</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-    </row>
-    <row r="55" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A55" s="4">
-        <v>742</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-    </row>
-    <row r="56" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A56" s="4">
-        <v>752</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-    </row>
-    <row r="57" spans="1:9" ht="99" x14ac:dyDescent="0.3">
-      <c r="A57" s="4">
-        <v>898</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G57" s="5" t="s">
+      <c r="D56" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-    </row>
-    <row r="58" spans="1:9" ht="99" x14ac:dyDescent="0.3">
-      <c r="A58" s="4">
-        <v>897</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
+      <c r="H56" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>